<commit_message>
add t_viv_col to report
</commit_message>
<xml_diff>
--- a/visorcarto/web/input/mnz_report.xlsx
+++ b/visorcarto/web/input/mnz_report.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects2020\ine\github\visorgis\visorcarto\web\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255F3441-E9BE-4ED7-8B69-585D911326D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte de Manzanos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Reporte de Manzanos Seleccionados</t>
   </si>
@@ -62,12 +61,15 @@
   </si>
   <si>
     <t>T_VIV_OCU</t>
+  </si>
+  <si>
+    <t>T_VIV_COL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -175,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -184,6 +186,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -227,7 +230,7 @@
         <xdr:cNvPr id="2" name="test_img" descr="test_img">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -542,12 +545,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,69 +564,75 @@
     <col min="7" max="7" width="16.42578125" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="15" style="5" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -655,13 +664,16 @@
         <v>11</v>
       </c>
       <c r="K5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -674,37 +686,39 @@
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B1:E4"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="F1:L4"/>
+    <mergeCell ref="A8:M8"/>
+    <mergeCell ref="F1:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>